<commit_message>
Changed logic for start and end time
Amended code to account for Start time & end time:
If this duration is greater than lunch break, there is a possibility that the driver will go for lunch. When this happens, we deduct lunch break from end time to prevent situation of exceeding 6pm from happening.
If this duration is less than lunch break, there is no way driver will go for lunch (or have a situation exceeding 6pm). Hence we do not deduct lunch break from end time.

This is to account for a solution that takes into consideration of customer's requested delivery time window - specifically Node 3 customer with delivery time 1600 to 1700, only 1 hr timeframe.
</commit_message>
<xml_diff>
--- a/Modelling_Using_Python1_clean - Copy (1).xlsx
+++ b/Modelling_Using_Python1_clean - Copy (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu.sharepoint.com/sites/FinalYearProject725/Shared Documents/General/1_Inputs/Full Data Cleaning and Analysis/Top 18 Customers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/138f29dc569e6e2b/Documents/MSC - Supply Chain Management/LI5001 Research Project/Data/Edit 9 - SAVINGS - 0904/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="11_F625815906C07340FE2A14EE3FDE99893451DC35" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A46911-9C1E-4028-B6B8-FD449CF2A618}"/>
+  <xr:revisionPtr revIDLastSave="396" documentId="11_F625815906C07340FE2A14EE3FDE99893451DC35" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87D53702-9367-474E-829F-6F88A4513F8E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distance Database" sheetId="6" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
   <si>
     <t>Factor</t>
   </si>
@@ -161,12 +161,6 @@
     <t>KM</t>
   </si>
   <si>
-    <t>Speed (&gt;150km)</t>
-  </si>
-  <si>
-    <t>Speed (&lt;=150km)</t>
-  </si>
-  <si>
     <t>이솝(금천가산)</t>
   </si>
   <si>
@@ -278,32 +272,31 @@
     <t>127.5263855,37.260333</t>
   </si>
   <si>
-    <t>Earliest Start Recess Time</t>
-  </si>
-  <si>
-    <t>HH:MM</t>
-  </si>
-  <si>
-    <t>Latest End Recess Time</t>
+    <t>Max Truck Size</t>
+  </si>
+  <si>
+    <t>Rates, KRW</t>
+  </si>
+  <si>
+    <t>Speed (&gt;70km)</t>
+  </si>
+  <si>
+    <t>Speed (&lt;=70km)</t>
   </si>
   <si>
     <t>Recess Length</t>
   </si>
   <si>
-    <t>Max Truck Size</t>
-  </si>
-  <si>
-    <t>Rates, KRW</t>
+    <t>Allowed Waiting Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
-    <numFmt numFmtId="166" formatCode="[$-14809]hh:mm;@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -394,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -489,15 +482,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="8"/>
       </left>
       <right/>
@@ -570,25 +554,19 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -596,9 +574,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -611,20 +586,39 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1858,95 +1852,95 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="34.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.86328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.19921875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.1328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.19921875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.9296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.9296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.53125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.9296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.86328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.19921875" style="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.86328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.19921875" style="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.53125" style="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.06640625" style="23"/>
+    <col min="1" max="1" width="5.453125" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="34.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="45" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" style="45" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.54296875" style="45" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="45" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7265625" style="45" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.81640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.81640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.81640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.81640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.1796875" style="45" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.54296875" style="45" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="29">
+      <c r="E1" s="44">
         <v>1</v>
       </c>
-      <c r="F1" s="29">
+      <c r="F1" s="44">
         <v>2</v>
       </c>
-      <c r="G1" s="29">
+      <c r="G1" s="44">
         <v>3</v>
       </c>
-      <c r="H1" s="29">
+      <c r="H1" s="44">
         <v>4</v>
       </c>
-      <c r="I1" s="29">
+      <c r="I1" s="44">
         <v>5</v>
       </c>
-      <c r="J1" s="29">
+      <c r="J1" s="44">
         <v>6</v>
       </c>
-      <c r="K1" s="29">
+      <c r="K1" s="44">
         <v>7</v>
       </c>
-      <c r="L1" s="29">
+      <c r="L1" s="44">
         <v>8</v>
       </c>
-      <c r="M1" s="29">
+      <c r="M1" s="44">
         <v>9</v>
       </c>
-      <c r="N1" s="29">
+      <c r="N1" s="44">
         <v>10</v>
       </c>
-      <c r="O1" s="29">
+      <c r="O1" s="44">
         <v>11</v>
       </c>
-      <c r="P1" s="29">
+      <c r="P1" s="44">
         <v>12</v>
       </c>
-      <c r="Q1" s="29">
+      <c r="Q1" s="44">
         <v>13</v>
       </c>
-      <c r="R1" s="29">
+      <c r="R1" s="44">
         <v>14</v>
       </c>
-      <c r="S1" s="29">
+      <c r="S1" s="44">
         <v>15</v>
       </c>
-      <c r="T1" s="29">
+      <c r="T1" s="44">
         <v>16</v>
       </c>
-      <c r="U1" s="29">
+      <c r="U1" s="44">
         <v>17</v>
       </c>
-      <c r="V1" s="29">
+      <c r="V1" s="44">
         <v>18</v>
       </c>
     </row>
@@ -1957,1420 +1951,1420 @@
       <c r="B2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="H2" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="I2" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="J2" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="K2" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="L2" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="M2" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="N2" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="O2" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="P2" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="Q2" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="R2" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="S2" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="32" t="s">
+      <c r="T2" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="U2" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="V2" s="46" t="s">
         <v>50</v>
-      </c>
-      <c r="U2" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="32" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="50"/>
       <c r="B3" s="50"/>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="F3" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="G3" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="H3" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="I3" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="J3" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="K3" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="L3" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="M3" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="N3" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="O3" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="P3" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="Q3" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="S3" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="T3" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="U3" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" s="47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="45">
+        <v>0</v>
+      </c>
+      <c r="E4" s="45">
+        <v>45.24</v>
+      </c>
+      <c r="F4" s="45">
+        <v>344.94</v>
+      </c>
+      <c r="G4" s="45">
+        <v>48.28</v>
+      </c>
+      <c r="H4" s="45">
+        <v>13.35</v>
+      </c>
+      <c r="I4" s="45">
+        <v>37.46</v>
+      </c>
+      <c r="J4" s="45">
+        <v>44.02</v>
+      </c>
+      <c r="K4" s="45">
+        <v>51.07</v>
+      </c>
+      <c r="L4" s="45">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="M4" s="45">
+        <v>29.33</v>
+      </c>
+      <c r="N4" s="45">
+        <v>5.35</v>
+      </c>
+      <c r="O4" s="45">
+        <v>59.71</v>
+      </c>
+      <c r="P4" s="45">
+        <v>337.3</v>
+      </c>
+      <c r="Q4" s="45">
+        <v>44.02</v>
+      </c>
+      <c r="R4" s="45">
+        <v>3.16</v>
+      </c>
+      <c r="S4" s="45">
+        <v>43.99</v>
+      </c>
+      <c r="T4" s="45">
+        <v>45.21</v>
+      </c>
+      <c r="U4" s="45">
+        <v>108.71</v>
+      </c>
+      <c r="V4" s="45">
+        <v>57.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="44">
+        <v>1</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="45">
+        <v>45.4</v>
+      </c>
+      <c r="E5" s="45">
+        <v>0</v>
+      </c>
+      <c r="F5" s="45">
+        <v>388.19</v>
+      </c>
+      <c r="G5" s="45">
+        <v>10.63</v>
+      </c>
+      <c r="H5" s="45">
+        <v>36.68</v>
+      </c>
+      <c r="I5" s="45">
+        <v>59.46</v>
+      </c>
+      <c r="J5" s="45">
+        <v>66.02</v>
+      </c>
+      <c r="K5" s="45">
+        <v>73.069999999999993</v>
+      </c>
+      <c r="L5" s="45">
+        <v>29.65</v>
+      </c>
+      <c r="M5" s="45">
+        <v>19.04</v>
+      </c>
+      <c r="N5" s="45">
+        <v>57</v>
+      </c>
+      <c r="O5" s="45">
+        <v>8.69</v>
+      </c>
+      <c r="P5" s="45">
+        <v>380.54</v>
+      </c>
+      <c r="Q5" s="45">
+        <v>66.02</v>
+      </c>
+      <c r="R5" s="45">
+        <v>47.68</v>
+      </c>
+      <c r="S5" s="45">
+        <v>1.45</v>
+      </c>
+      <c r="T5" s="45">
+        <v>0.48</v>
+      </c>
+      <c r="U5" s="45">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="V5" s="45">
+        <v>70.55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="44">
+        <v>2</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="45">
+        <v>345.7</v>
+      </c>
+      <c r="E6" s="45">
+        <v>387.98</v>
+      </c>
+      <c r="F6" s="45">
+        <v>0</v>
+      </c>
+      <c r="G6" s="45">
+        <v>384.39</v>
+      </c>
+      <c r="H6" s="45">
+        <v>356.71</v>
+      </c>
+      <c r="I6" s="45">
+        <v>334.45</v>
+      </c>
+      <c r="J6" s="45">
+        <v>328.23</v>
+      </c>
+      <c r="K6" s="45">
+        <v>320.56</v>
+      </c>
+      <c r="L6" s="45">
+        <v>419.11</v>
+      </c>
+      <c r="M6" s="45">
+        <v>372.07</v>
+      </c>
+      <c r="N6" s="45">
+        <v>350.84</v>
+      </c>
+      <c r="O6" s="45">
+        <v>395.82</v>
+      </c>
+      <c r="P6" s="45">
+        <v>21.49</v>
+      </c>
+      <c r="Q6" s="45">
+        <v>328.23</v>
+      </c>
+      <c r="R6" s="45">
+        <v>347.27</v>
+      </c>
+      <c r="S6" s="45">
+        <v>386.73</v>
+      </c>
+      <c r="T6" s="45">
+        <v>387.95</v>
+      </c>
+      <c r="U6" s="45">
+        <v>252.82</v>
+      </c>
+      <c r="V6" s="45">
+        <v>320.35000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="44">
+        <v>3</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="45">
+        <v>46.94</v>
+      </c>
+      <c r="E7" s="45">
+        <v>12.56</v>
+      </c>
+      <c r="F7" s="45">
+        <v>383.86</v>
+      </c>
+      <c r="G7" s="45">
+        <v>0</v>
+      </c>
+      <c r="H7" s="45">
+        <v>40.89</v>
+      </c>
+      <c r="I7" s="45">
+        <v>55.13</v>
+      </c>
+      <c r="J7" s="45">
+        <v>61.69</v>
+      </c>
+      <c r="K7" s="45">
+        <v>68.739999999999995</v>
+      </c>
+      <c r="L7" s="45">
+        <v>35.94</v>
+      </c>
+      <c r="M7" s="45">
+        <v>19.93</v>
+      </c>
+      <c r="N7" s="45">
+        <v>52.08</v>
+      </c>
+      <c r="O7" s="45">
+        <v>12.35</v>
+      </c>
+      <c r="P7" s="45">
+        <v>376.22</v>
+      </c>
+      <c r="Q7" s="45">
+        <v>61.69</v>
+      </c>
+      <c r="R7" s="45">
+        <v>48.51</v>
+      </c>
+      <c r="S7" s="45">
+        <v>13.49</v>
+      </c>
+      <c r="T7" s="45">
+        <v>12.32</v>
+      </c>
+      <c r="U7" s="45">
+        <v>152.63</v>
+      </c>
+      <c r="V7" s="45">
+        <v>62.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="44">
+        <v>4</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="45">
+        <v>13.31</v>
+      </c>
+      <c r="E8" s="45">
+        <v>36.520000000000003</v>
+      </c>
+      <c r="F8" s="45">
+        <v>355.42</v>
+      </c>
+      <c r="G8" s="45">
+        <v>41.49</v>
+      </c>
+      <c r="H8" s="45">
+        <v>0</v>
+      </c>
+      <c r="I8" s="45">
+        <v>36.14</v>
+      </c>
+      <c r="J8" s="45">
+        <v>42.71</v>
+      </c>
+      <c r="K8" s="45">
+        <v>49.76</v>
+      </c>
+      <c r="L8" s="45">
+        <v>65.180000000000007</v>
+      </c>
+      <c r="M8" s="45">
+        <v>20.61</v>
+      </c>
+      <c r="N8" s="45">
+        <v>18.36</v>
+      </c>
+      <c r="O8" s="45">
+        <v>44.93</v>
+      </c>
+      <c r="P8" s="45">
+        <v>347.78</v>
+      </c>
+      <c r="Q8" s="45">
+        <v>42.71</v>
+      </c>
+      <c r="R8" s="45">
+        <v>14.77</v>
+      </c>
+      <c r="S8" s="45">
+        <v>35.26</v>
+      </c>
+      <c r="T8" s="45">
+        <v>36.49</v>
+      </c>
+      <c r="U8" s="45">
+        <v>119.19</v>
+      </c>
+      <c r="V8" s="45">
+        <v>56.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="44">
+        <v>5</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="45">
+        <v>38.369999999999997</v>
+      </c>
+      <c r="E9" s="45">
+        <v>59.09</v>
+      </c>
+      <c r="F9" s="45">
+        <v>334.07</v>
+      </c>
+      <c r="G9" s="45">
+        <v>55.49</v>
+      </c>
+      <c r="H9" s="45">
+        <v>36.96</v>
+      </c>
+      <c r="I9" s="45">
+        <v>0</v>
+      </c>
+      <c r="J9" s="45">
+        <v>7.36</v>
+      </c>
+      <c r="K9" s="45">
+        <v>14.41</v>
+      </c>
+      <c r="L9" s="45">
+        <v>90.21</v>
+      </c>
+      <c r="M9" s="45">
+        <v>43.18</v>
+      </c>
+      <c r="N9" s="45">
+        <v>43.51</v>
+      </c>
+      <c r="O9" s="45">
+        <v>66.92</v>
+      </c>
+      <c r="P9" s="45">
+        <v>326.42</v>
+      </c>
+      <c r="Q9" s="45">
+        <v>7.36</v>
+      </c>
+      <c r="R9" s="45">
+        <v>39.94</v>
+      </c>
+      <c r="S9" s="45">
+        <v>57.83</v>
+      </c>
+      <c r="T9" s="45">
+        <v>59.05</v>
+      </c>
+      <c r="U9" s="45">
+        <v>108.03</v>
+      </c>
+      <c r="V9" s="45">
+        <v>35.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="44">
+        <v>6</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="45">
+        <v>45.06</v>
+      </c>
+      <c r="E10" s="45">
+        <v>65.77</v>
+      </c>
+      <c r="F10" s="45">
+        <v>327.67</v>
+      </c>
+      <c r="G10" s="45">
+        <v>62.18</v>
+      </c>
+      <c r="H10" s="45">
+        <v>43.65</v>
+      </c>
+      <c r="I10" s="45">
+        <v>7.34</v>
+      </c>
+      <c r="J10" s="45">
+        <v>0</v>
+      </c>
+      <c r="K10" s="45">
+        <v>8.01</v>
+      </c>
+      <c r="L10" s="45">
+        <v>96.9</v>
+      </c>
+      <c r="M10" s="45">
+        <v>49.86</v>
+      </c>
+      <c r="N10" s="45">
+        <v>50.2</v>
+      </c>
+      <c r="O10" s="45">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="P10" s="45">
+        <v>320.02999999999997</v>
+      </c>
+      <c r="Q10" s="45">
+        <v>0</v>
+      </c>
+      <c r="R10" s="45">
+        <v>46.63</v>
+      </c>
+      <c r="S10" s="45">
+        <v>64.510000000000005</v>
+      </c>
+      <c r="T10" s="45">
+        <v>65.73</v>
+      </c>
+      <c r="U10" s="45">
+        <v>101.64</v>
+      </c>
+      <c r="V10" s="45">
+        <v>27.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="44">
+        <v>7</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="45">
+        <v>52.16</v>
+      </c>
+      <c r="E11" s="45">
+        <v>72.88</v>
+      </c>
+      <c r="F11" s="45">
+        <v>320.27</v>
+      </c>
+      <c r="G11" s="45">
+        <v>69.28</v>
+      </c>
+      <c r="H11" s="45">
+        <v>50.76</v>
+      </c>
+      <c r="I11" s="45">
+        <v>14.45</v>
+      </c>
+      <c r="J11" s="45">
+        <v>8.23</v>
+      </c>
+      <c r="K11" s="45">
+        <v>0</v>
+      </c>
+      <c r="L11" s="45">
+        <v>104.01</v>
+      </c>
+      <c r="M11" s="45">
+        <v>56.97</v>
+      </c>
+      <c r="N11" s="45">
+        <v>57.31</v>
+      </c>
+      <c r="O11" s="45">
+        <v>80.709999999999994</v>
+      </c>
+      <c r="P11" s="45">
+        <v>312.63</v>
+      </c>
+      <c r="Q11" s="45">
+        <v>8.23</v>
+      </c>
+      <c r="R11" s="45">
+        <v>53.73</v>
+      </c>
+      <c r="S11" s="45">
+        <v>71.62</v>
+      </c>
+      <c r="T11" s="45">
+        <v>72.84</v>
+      </c>
+      <c r="U11" s="45">
+        <v>94.24</v>
+      </c>
+      <c r="V11" s="45">
+        <v>24.97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="44">
+        <v>8</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="34" t="s">
+      <c r="D12" s="45">
+        <v>72.349999999999994</v>
+      </c>
+      <c r="E12" s="45">
+        <v>29.03</v>
+      </c>
+      <c r="F12" s="45">
+        <v>416.7</v>
+      </c>
+      <c r="G12" s="45">
+        <v>36.11</v>
+      </c>
+      <c r="H12" s="45">
+        <v>63.63</v>
+      </c>
+      <c r="I12" s="45">
+        <v>87.97</v>
+      </c>
+      <c r="J12" s="45">
+        <v>94.54</v>
+      </c>
+      <c r="K12" s="45">
+        <v>101.58</v>
+      </c>
+      <c r="L12" s="45">
+        <v>0</v>
+      </c>
+      <c r="M12" s="45">
+        <v>46.8</v>
+      </c>
+      <c r="N12" s="45">
+        <v>83</v>
+      </c>
+      <c r="O12" s="45">
+        <v>27.15</v>
+      </c>
+      <c r="P12" s="45">
+        <v>409.06</v>
+      </c>
+      <c r="Q12" s="45">
+        <v>94.54</v>
+      </c>
+      <c r="R12" s="45">
+        <v>74.64</v>
+      </c>
+      <c r="S12" s="45">
+        <v>28.84</v>
+      </c>
+      <c r="T12" s="45">
+        <v>29</v>
+      </c>
+      <c r="U12" s="45">
+        <v>185.62</v>
+      </c>
+      <c r="V12" s="45">
+        <v>98.16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="44">
+        <v>9</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="45">
+        <v>29.33</v>
+      </c>
+      <c r="E13" s="45">
+        <v>18.95</v>
+      </c>
+      <c r="F13" s="45">
+        <v>372.11</v>
+      </c>
+      <c r="G13" s="45">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H13" s="45">
+        <v>20.61</v>
+      </c>
+      <c r="I13" s="45">
+        <v>43.38</v>
+      </c>
+      <c r="J13" s="45">
+        <v>49.95</v>
+      </c>
+      <c r="K13" s="45">
+        <v>56.99</v>
+      </c>
+      <c r="L13" s="45">
+        <v>47.88</v>
+      </c>
+      <c r="M13" s="45">
+        <v>0</v>
+      </c>
+      <c r="N13" s="45">
+        <v>38.659999999999997</v>
+      </c>
+      <c r="O13" s="45">
+        <v>27.36</v>
+      </c>
+      <c r="P13" s="45">
+        <v>364.47</v>
+      </c>
+      <c r="Q13" s="45">
+        <v>49.95</v>
+      </c>
+      <c r="R13" s="45">
+        <v>31.61</v>
+      </c>
+      <c r="S13" s="45">
+        <v>17.7</v>
+      </c>
+      <c r="T13" s="45">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="U13" s="45">
+        <v>141.03</v>
+      </c>
+      <c r="V13" s="45">
+        <v>63.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="44">
+        <v>10</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="45">
+        <v>5.31</v>
+      </c>
+      <c r="E14" s="45">
+        <v>53.72</v>
+      </c>
+      <c r="F14" s="45">
+        <v>350.02</v>
+      </c>
+      <c r="G14" s="45">
+        <v>53.36</v>
+      </c>
+      <c r="H14" s="45">
+        <v>18.36</v>
+      </c>
+      <c r="I14" s="45">
+        <v>42.54</v>
+      </c>
+      <c r="J14" s="45">
+        <v>49.1</v>
+      </c>
+      <c r="K14" s="45">
+        <v>56.15</v>
+      </c>
+      <c r="L14" s="45">
+        <v>82.05</v>
+      </c>
+      <c r="M14" s="45">
+        <v>35.01</v>
+      </c>
+      <c r="N14" s="45">
+        <v>0</v>
+      </c>
+      <c r="O14" s="45">
+        <v>62.13</v>
+      </c>
+      <c r="P14" s="45">
+        <v>342.38</v>
+      </c>
+      <c r="Q14" s="45">
+        <v>49.1</v>
+      </c>
+      <c r="R14" s="45">
+        <v>5.37</v>
+      </c>
+      <c r="S14" s="45">
+        <v>52.47</v>
+      </c>
+      <c r="T14" s="45">
+        <v>53.69</v>
+      </c>
+      <c r="U14" s="45">
+        <v>113.79</v>
+      </c>
+      <c r="V14" s="45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="44">
+        <v>11</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="45">
+        <v>58.07</v>
+      </c>
+      <c r="E15" s="45">
+        <v>9.02</v>
+      </c>
+      <c r="F15" s="45">
+        <v>394.98</v>
+      </c>
+      <c r="G15" s="45">
+        <v>11.61</v>
+      </c>
+      <c r="H15" s="45">
+        <v>52.02</v>
+      </c>
+      <c r="I15" s="45">
+        <v>66.260000000000005</v>
+      </c>
+      <c r="J15" s="45">
+        <v>72.819999999999993</v>
+      </c>
+      <c r="K15" s="45">
+        <v>79.87</v>
+      </c>
+      <c r="L15" s="45">
+        <v>27.57</v>
+      </c>
+      <c r="M15" s="45">
+        <v>28.24</v>
+      </c>
+      <c r="N15" s="45">
+        <v>63.21</v>
+      </c>
+      <c r="O15" s="45">
+        <v>0</v>
+      </c>
+      <c r="P15" s="45">
+        <v>387.34</v>
+      </c>
+      <c r="Q15" s="45">
+        <v>72.819999999999993</v>
+      </c>
+      <c r="R15" s="45">
+        <v>59.64</v>
+      </c>
+      <c r="S15" s="45">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="T15" s="45">
+        <v>8.6</v>
+      </c>
+      <c r="U15" s="45">
+        <v>163.75</v>
+      </c>
+      <c r="V15" s="45">
+        <v>73.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="44">
+        <v>12</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="45">
+        <v>337.26</v>
+      </c>
+      <c r="E16" s="45">
+        <v>379.54</v>
+      </c>
+      <c r="F16" s="45">
+        <v>22.6</v>
+      </c>
+      <c r="G16" s="45">
+        <v>375.95</v>
+      </c>
+      <c r="H16" s="45">
+        <v>348.27</v>
+      </c>
+      <c r="I16" s="45">
+        <v>326.01</v>
+      </c>
+      <c r="J16" s="45">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="K16" s="45">
+        <v>312.12</v>
+      </c>
+      <c r="L16" s="45">
+        <v>410.67</v>
+      </c>
+      <c r="M16" s="45">
+        <v>363.63</v>
+      </c>
+      <c r="N16" s="45">
+        <v>342.4</v>
+      </c>
+      <c r="O16" s="45">
+        <v>387.38</v>
+      </c>
+      <c r="P16" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="45">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="R16" s="45">
+        <v>338.83</v>
+      </c>
+      <c r="S16" s="45">
+        <v>378.29</v>
+      </c>
+      <c r="T16" s="45">
+        <v>379.51</v>
+      </c>
+      <c r="U16" s="45">
+        <v>234.98</v>
+      </c>
+      <c r="V16" s="45">
+        <v>311.91000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="44">
+        <v>13</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="45">
+        <v>45.06</v>
+      </c>
+      <c r="E17" s="45">
+        <v>65.77</v>
+      </c>
+      <c r="F17" s="45">
+        <v>327.67</v>
+      </c>
+      <c r="G17" s="45">
+        <v>62.18</v>
+      </c>
+      <c r="H17" s="45">
+        <v>43.65</v>
+      </c>
+      <c r="I17" s="45">
+        <v>7.34</v>
+      </c>
+      <c r="J17" s="45">
+        <v>0</v>
+      </c>
+      <c r="K17" s="45">
+        <v>8.01</v>
+      </c>
+      <c r="L17" s="45">
+        <v>96.9</v>
+      </c>
+      <c r="M17" s="45">
+        <v>49.86</v>
+      </c>
+      <c r="N17" s="45">
+        <v>50.2</v>
+      </c>
+      <c r="O17" s="45">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="P17" s="45">
+        <v>320.02999999999997</v>
+      </c>
+      <c r="Q17" s="45">
+        <v>0</v>
+      </c>
+      <c r="R17" s="45">
+        <v>46.63</v>
+      </c>
+      <c r="S17" s="45">
+        <v>64.510000000000005</v>
+      </c>
+      <c r="T17" s="45">
+        <v>65.73</v>
+      </c>
+      <c r="U17" s="45">
+        <v>101.64</v>
+      </c>
+      <c r="V17" s="45">
+        <v>27.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="44">
+        <v>14</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="45">
+        <v>3.17</v>
+      </c>
+      <c r="E18" s="45">
+        <v>47.52</v>
+      </c>
+      <c r="F18" s="45">
+        <v>346.47</v>
+      </c>
+      <c r="G18" s="45">
+        <v>49.81</v>
+      </c>
+      <c r="H18" s="45">
+        <v>14.79</v>
+      </c>
+      <c r="I18" s="45">
+        <v>38.99</v>
+      </c>
+      <c r="J18" s="45">
+        <v>45.55</v>
+      </c>
+      <c r="K18" s="45">
+        <v>52.6</v>
+      </c>
+      <c r="L18" s="45">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="M18" s="45">
+        <v>31.61</v>
+      </c>
+      <c r="N18" s="45">
+        <v>5.14</v>
+      </c>
+      <c r="O18" s="45">
+        <v>61.24</v>
+      </c>
+      <c r="P18" s="45">
+        <v>338.83</v>
+      </c>
+      <c r="Q18" s="45">
+        <v>45.55</v>
+      </c>
+      <c r="R18" s="45">
+        <v>0</v>
+      </c>
+      <c r="S18" s="45">
+        <v>46.27</v>
+      </c>
+      <c r="T18" s="45">
+        <v>47.49</v>
+      </c>
+      <c r="U18" s="45">
+        <v>110.24</v>
+      </c>
+      <c r="V18" s="45">
+        <v>59.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="44">
+        <v>15</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="45">
+        <v>44.1</v>
+      </c>
+      <c r="E19" s="45">
+        <v>1.72</v>
+      </c>
+      <c r="F19" s="45">
+        <v>386.88</v>
+      </c>
+      <c r="G19" s="45">
+        <v>11.82</v>
+      </c>
+      <c r="H19" s="45">
+        <v>35.369999999999997</v>
+      </c>
+      <c r="I19" s="45">
+        <v>58.15</v>
+      </c>
+      <c r="J19" s="45">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="K19" s="45">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="L19" s="45">
+        <v>29.13</v>
+      </c>
+      <c r="M19" s="45">
+        <v>17.73</v>
+      </c>
+      <c r="N19" s="45">
+        <v>56.94</v>
+      </c>
+      <c r="O19" s="45">
+        <v>9.58</v>
+      </c>
+      <c r="P19" s="45">
+        <v>379.24</v>
+      </c>
+      <c r="Q19" s="45">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="R19" s="45">
+        <v>46.38</v>
+      </c>
+      <c r="S19" s="45">
+        <v>0</v>
+      </c>
+      <c r="T19" s="45">
+        <v>1.68</v>
+      </c>
+      <c r="U19" s="45">
+        <v>162.63999999999999</v>
+      </c>
+      <c r="V19" s="45">
+        <v>74.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="44">
+        <v>16</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="D20" s="45">
+        <v>45.51</v>
+      </c>
+      <c r="E20" s="45">
+        <v>0.62</v>
+      </c>
+      <c r="F20" s="45">
+        <v>388.29</v>
+      </c>
+      <c r="G20" s="45">
+        <v>12.28</v>
+      </c>
+      <c r="H20" s="45">
+        <v>36.78</v>
+      </c>
+      <c r="I20" s="45">
+        <v>59.56</v>
+      </c>
+      <c r="J20" s="45">
+        <v>66.12</v>
+      </c>
+      <c r="K20" s="45">
+        <v>73.17</v>
+      </c>
+      <c r="L20" s="45">
+        <v>29.23</v>
+      </c>
+      <c r="M20" s="45">
+        <v>19.14</v>
+      </c>
+      <c r="N20" s="45">
+        <v>57.1</v>
+      </c>
+      <c r="O20" s="45">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="P20" s="45">
+        <v>380.65</v>
+      </c>
+      <c r="Q20" s="45">
+        <v>66.12</v>
+      </c>
+      <c r="R20" s="45">
+        <v>47.79</v>
+      </c>
+      <c r="S20" s="45">
+        <v>1.55</v>
+      </c>
+      <c r="T20" s="45">
+        <v>0</v>
+      </c>
+      <c r="U20" s="45">
+        <v>162.80000000000001</v>
+      </c>
+      <c r="V20" s="45">
+        <v>70.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="44">
+        <v>17</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="D21" s="45">
+        <v>108.77</v>
+      </c>
+      <c r="E21" s="45">
+        <v>163</v>
+      </c>
+      <c r="F21" s="45">
+        <v>251.96</v>
+      </c>
+      <c r="G21" s="45">
+        <v>153.21</v>
+      </c>
+      <c r="H21" s="45">
+        <v>119.78</v>
+      </c>
+      <c r="I21" s="45">
+        <v>108.25</v>
+      </c>
+      <c r="J21" s="45">
+        <v>102.03</v>
+      </c>
+      <c r="K21" s="45">
+        <v>94.36</v>
+      </c>
+      <c r="L21" s="45">
+        <v>191.33</v>
+      </c>
+      <c r="M21" s="45">
+        <v>136.86000000000001</v>
+      </c>
+      <c r="N21" s="45">
+        <v>113.91</v>
+      </c>
+      <c r="O21" s="45">
+        <v>164.64</v>
+      </c>
+      <c r="P21" s="45">
+        <v>235.16</v>
+      </c>
+      <c r="Q21" s="45">
+        <v>102.03</v>
+      </c>
+      <c r="R21" s="45">
+        <v>110.34</v>
+      </c>
+      <c r="S21" s="45">
+        <v>161.75</v>
+      </c>
+      <c r="T21" s="45">
+        <v>162.97</v>
+      </c>
+      <c r="U21" s="45">
+        <v>0</v>
+      </c>
+      <c r="V21" s="45">
+        <v>120.34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="44">
+        <v>18</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" s="34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="23">
-        <v>0</v>
-      </c>
-      <c r="E4" s="23">
-        <v>45.24</v>
-      </c>
-      <c r="F4" s="23">
-        <v>344.94</v>
-      </c>
-      <c r="G4" s="23">
-        <v>48.28</v>
-      </c>
-      <c r="H4" s="23">
-        <v>13.35</v>
-      </c>
-      <c r="I4" s="23">
-        <v>37.46</v>
-      </c>
-      <c r="J4" s="23">
-        <v>44.02</v>
-      </c>
-      <c r="K4" s="23">
-        <v>51.07</v>
-      </c>
-      <c r="L4" s="23">
-        <v>73.900000000000006</v>
-      </c>
-      <c r="M4" s="23">
-        <v>29.33</v>
-      </c>
-      <c r="N4" s="23">
-        <v>5.35</v>
-      </c>
-      <c r="O4" s="23">
-        <v>59.71</v>
-      </c>
-      <c r="P4" s="23">
-        <v>337.3</v>
-      </c>
-      <c r="Q4" s="23">
-        <v>44.02</v>
-      </c>
-      <c r="R4" s="23">
-        <v>3.16</v>
-      </c>
-      <c r="S4" s="23">
-        <v>43.99</v>
-      </c>
-      <c r="T4" s="23">
-        <v>45.21</v>
-      </c>
-      <c r="U4" s="23">
-        <v>108.71</v>
-      </c>
-      <c r="V4" s="23">
-        <v>57.92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="29">
-        <v>1</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="23">
-        <v>45.4</v>
-      </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23">
-        <v>388.19</v>
-      </c>
-      <c r="G5" s="23">
-        <v>10.63</v>
-      </c>
-      <c r="H5" s="23">
-        <v>36.68</v>
-      </c>
-      <c r="I5" s="23">
-        <v>59.46</v>
-      </c>
-      <c r="J5" s="23">
-        <v>66.02</v>
-      </c>
-      <c r="K5" s="23">
-        <v>73.069999999999993</v>
-      </c>
-      <c r="L5" s="23">
-        <v>29.65</v>
-      </c>
-      <c r="M5" s="23">
-        <v>19.04</v>
-      </c>
-      <c r="N5" s="23">
-        <v>57</v>
-      </c>
-      <c r="O5" s="23">
-        <v>8.69</v>
-      </c>
-      <c r="P5" s="23">
-        <v>380.54</v>
-      </c>
-      <c r="Q5" s="23">
-        <v>66.02</v>
-      </c>
-      <c r="R5" s="23">
-        <v>47.68</v>
-      </c>
-      <c r="S5" s="23">
-        <v>1.45</v>
-      </c>
-      <c r="T5" s="23">
-        <v>0.48</v>
-      </c>
-      <c r="U5" s="23">
-        <v>162.69999999999999</v>
-      </c>
-      <c r="V5" s="23">
-        <v>70.55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="29">
-        <v>2</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="23">
-        <v>345.7</v>
-      </c>
-      <c r="E6" s="23">
-        <v>387.98</v>
-      </c>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-      <c r="G6" s="23">
-        <v>384.39</v>
-      </c>
-      <c r="H6" s="23">
-        <v>356.71</v>
-      </c>
-      <c r="I6" s="23">
-        <v>334.45</v>
-      </c>
-      <c r="J6" s="23">
-        <v>328.23</v>
-      </c>
-      <c r="K6" s="23">
-        <v>320.56</v>
-      </c>
-      <c r="L6" s="23">
-        <v>419.11</v>
-      </c>
-      <c r="M6" s="23">
-        <v>372.07</v>
-      </c>
-      <c r="N6" s="23">
-        <v>350.84</v>
-      </c>
-      <c r="O6" s="23">
-        <v>395.82</v>
-      </c>
-      <c r="P6" s="23">
-        <v>21.49</v>
-      </c>
-      <c r="Q6" s="23">
-        <v>328.23</v>
-      </c>
-      <c r="R6" s="23">
-        <v>347.27</v>
-      </c>
-      <c r="S6" s="23">
-        <v>386.73</v>
-      </c>
-      <c r="T6" s="23">
-        <v>387.95</v>
-      </c>
-      <c r="U6" s="23">
-        <v>252.82</v>
-      </c>
-      <c r="V6" s="23">
-        <v>320.35000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="29">
-        <v>3</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="23">
-        <v>46.94</v>
-      </c>
-      <c r="E7" s="23">
-        <v>12.56</v>
-      </c>
-      <c r="F7" s="23">
-        <v>383.86</v>
-      </c>
-      <c r="G7" s="23">
-        <v>0</v>
-      </c>
-      <c r="H7" s="23">
-        <v>40.89</v>
-      </c>
-      <c r="I7" s="23">
-        <v>55.13</v>
-      </c>
-      <c r="J7" s="23">
-        <v>61.69</v>
-      </c>
-      <c r="K7" s="23">
-        <v>68.739999999999995</v>
-      </c>
-      <c r="L7" s="23">
-        <v>35.94</v>
-      </c>
-      <c r="M7" s="23">
-        <v>19.93</v>
-      </c>
-      <c r="N7" s="23">
-        <v>52.08</v>
-      </c>
-      <c r="O7" s="23">
-        <v>12.35</v>
-      </c>
-      <c r="P7" s="23">
-        <v>376.22</v>
-      </c>
-      <c r="Q7" s="23">
-        <v>61.69</v>
-      </c>
-      <c r="R7" s="23">
-        <v>48.51</v>
-      </c>
-      <c r="S7" s="23">
-        <v>13.49</v>
-      </c>
-      <c r="T7" s="23">
-        <v>12.32</v>
-      </c>
-      <c r="U7" s="23">
-        <v>152.63</v>
-      </c>
-      <c r="V7" s="23">
-        <v>62.91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="29">
-        <v>4</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="23">
-        <v>13.31</v>
-      </c>
-      <c r="E8" s="23">
-        <v>36.520000000000003</v>
-      </c>
-      <c r="F8" s="23">
-        <v>355.42</v>
-      </c>
-      <c r="G8" s="23">
-        <v>41.49</v>
-      </c>
-      <c r="H8" s="23">
-        <v>0</v>
-      </c>
-      <c r="I8" s="23">
-        <v>36.14</v>
-      </c>
-      <c r="J8" s="23">
-        <v>42.71</v>
-      </c>
-      <c r="K8" s="23">
-        <v>49.76</v>
-      </c>
-      <c r="L8" s="23">
-        <v>65.180000000000007</v>
-      </c>
-      <c r="M8" s="23">
-        <v>20.61</v>
-      </c>
-      <c r="N8" s="23">
-        <v>18.36</v>
-      </c>
-      <c r="O8" s="23">
-        <v>44.93</v>
-      </c>
-      <c r="P8" s="23">
-        <v>347.78</v>
-      </c>
-      <c r="Q8" s="23">
-        <v>42.71</v>
-      </c>
-      <c r="R8" s="23">
-        <v>14.77</v>
-      </c>
-      <c r="S8" s="23">
-        <v>35.26</v>
-      </c>
-      <c r="T8" s="23">
-        <v>36.49</v>
-      </c>
-      <c r="U8" s="23">
-        <v>119.19</v>
-      </c>
-      <c r="V8" s="23">
-        <v>56.61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="29">
-        <v>5</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="23">
-        <v>38.369999999999997</v>
-      </c>
-      <c r="E9" s="23">
-        <v>59.09</v>
-      </c>
-      <c r="F9" s="23">
-        <v>334.07</v>
-      </c>
-      <c r="G9" s="23">
-        <v>55.49</v>
-      </c>
-      <c r="H9" s="23">
-        <v>36.96</v>
-      </c>
-      <c r="I9" s="23">
-        <v>0</v>
-      </c>
-      <c r="J9" s="23">
-        <v>7.36</v>
-      </c>
-      <c r="K9" s="23">
-        <v>14.41</v>
-      </c>
-      <c r="L9" s="23">
-        <v>90.21</v>
-      </c>
-      <c r="M9" s="23">
-        <v>43.18</v>
-      </c>
-      <c r="N9" s="23">
-        <v>43.51</v>
-      </c>
-      <c r="O9" s="23">
-        <v>66.92</v>
-      </c>
-      <c r="P9" s="23">
-        <v>326.42</v>
-      </c>
-      <c r="Q9" s="23">
-        <v>7.36</v>
-      </c>
-      <c r="R9" s="23">
-        <v>39.94</v>
-      </c>
-      <c r="S9" s="23">
-        <v>57.83</v>
-      </c>
-      <c r="T9" s="23">
-        <v>59.05</v>
-      </c>
-      <c r="U9" s="23">
-        <v>108.03</v>
-      </c>
-      <c r="V9" s="23">
-        <v>35.29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="29">
-        <v>6</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="23">
-        <v>45.06</v>
-      </c>
-      <c r="E10" s="23">
-        <v>65.77</v>
-      </c>
-      <c r="F10" s="23">
-        <v>327.67</v>
-      </c>
-      <c r="G10" s="23">
-        <v>62.18</v>
-      </c>
-      <c r="H10" s="23">
-        <v>43.65</v>
-      </c>
-      <c r="I10" s="23">
-        <v>7.34</v>
-      </c>
-      <c r="J10" s="23">
-        <v>0</v>
-      </c>
-      <c r="K10" s="23">
-        <v>8.01</v>
-      </c>
-      <c r="L10" s="23">
-        <v>96.9</v>
-      </c>
-      <c r="M10" s="23">
-        <v>49.86</v>
-      </c>
-      <c r="N10" s="23">
-        <v>50.2</v>
-      </c>
-      <c r="O10" s="23">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="P10" s="23">
-        <v>320.02999999999997</v>
-      </c>
-      <c r="Q10" s="23">
-        <v>0</v>
-      </c>
-      <c r="R10" s="23">
-        <v>46.63</v>
-      </c>
-      <c r="S10" s="23">
-        <v>64.510000000000005</v>
-      </c>
-      <c r="T10" s="23">
-        <v>65.73</v>
-      </c>
-      <c r="U10" s="23">
-        <v>101.64</v>
-      </c>
-      <c r="V10" s="23">
-        <v>27.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="29">
-        <v>7</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="23">
-        <v>52.16</v>
-      </c>
-      <c r="E11" s="23">
-        <v>72.88</v>
-      </c>
-      <c r="F11" s="23">
-        <v>320.27</v>
-      </c>
-      <c r="G11" s="23">
-        <v>69.28</v>
-      </c>
-      <c r="H11" s="23">
-        <v>50.76</v>
-      </c>
-      <c r="I11" s="23">
-        <v>14.45</v>
-      </c>
-      <c r="J11" s="23">
-        <v>8.23</v>
-      </c>
-      <c r="K11" s="23">
-        <v>0</v>
-      </c>
-      <c r="L11" s="23">
-        <v>104.01</v>
-      </c>
-      <c r="M11" s="23">
-        <v>56.97</v>
-      </c>
-      <c r="N11" s="23">
-        <v>57.31</v>
-      </c>
-      <c r="O11" s="23">
-        <v>80.709999999999994</v>
-      </c>
-      <c r="P11" s="23">
-        <v>312.63</v>
-      </c>
-      <c r="Q11" s="23">
-        <v>8.23</v>
-      </c>
-      <c r="R11" s="23">
-        <v>53.73</v>
-      </c>
-      <c r="S11" s="23">
-        <v>71.62</v>
-      </c>
-      <c r="T11" s="23">
-        <v>72.84</v>
-      </c>
-      <c r="U11" s="23">
-        <v>94.24</v>
-      </c>
-      <c r="V11" s="23">
-        <v>24.97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="29">
-        <v>8</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="23">
-        <v>72.349999999999994</v>
-      </c>
-      <c r="E12" s="23">
-        <v>29.03</v>
-      </c>
-      <c r="F12" s="23">
-        <v>416.7</v>
-      </c>
-      <c r="G12" s="23">
-        <v>36.11</v>
-      </c>
-      <c r="H12" s="23">
-        <v>63.63</v>
-      </c>
-      <c r="I12" s="23">
-        <v>87.97</v>
-      </c>
-      <c r="J12" s="23">
-        <v>94.54</v>
-      </c>
-      <c r="K12" s="23">
-        <v>101.58</v>
-      </c>
-      <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23">
-        <v>46.8</v>
-      </c>
-      <c r="N12" s="23">
-        <v>83</v>
-      </c>
-      <c r="O12" s="23">
-        <v>27.15</v>
-      </c>
-      <c r="P12" s="23">
-        <v>409.06</v>
-      </c>
-      <c r="Q12" s="23">
-        <v>94.54</v>
-      </c>
-      <c r="R12" s="23">
-        <v>74.64</v>
-      </c>
-      <c r="S12" s="23">
-        <v>28.84</v>
-      </c>
-      <c r="T12" s="23">
-        <v>29</v>
-      </c>
-      <c r="U12" s="23">
-        <v>185.62</v>
-      </c>
-      <c r="V12" s="23">
-        <v>98.16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="29">
-        <v>9</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="23">
-        <v>29.33</v>
-      </c>
-      <c r="E13" s="23">
-        <v>18.95</v>
-      </c>
-      <c r="F13" s="23">
-        <v>372.11</v>
-      </c>
-      <c r="G13" s="23">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="H13" s="23">
-        <v>20.61</v>
-      </c>
-      <c r="I13" s="23">
-        <v>43.38</v>
-      </c>
-      <c r="J13" s="23">
-        <v>49.95</v>
-      </c>
-      <c r="K13" s="23">
-        <v>56.99</v>
-      </c>
-      <c r="L13" s="23">
-        <v>47.88</v>
-      </c>
-      <c r="M13" s="23">
-        <v>0</v>
-      </c>
-      <c r="N13" s="23">
-        <v>38.659999999999997</v>
-      </c>
-      <c r="O13" s="23">
-        <v>27.36</v>
-      </c>
-      <c r="P13" s="23">
-        <v>364.47</v>
-      </c>
-      <c r="Q13" s="23">
-        <v>49.95</v>
-      </c>
-      <c r="R13" s="23">
-        <v>31.61</v>
-      </c>
-      <c r="S13" s="23">
-        <v>17.7</v>
-      </c>
-      <c r="T13" s="23">
-        <v>18.920000000000002</v>
-      </c>
-      <c r="U13" s="23">
-        <v>141.03</v>
-      </c>
-      <c r="V13" s="23">
-        <v>63.85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="29">
-        <v>10</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="23">
-        <v>5.31</v>
-      </c>
-      <c r="E14" s="23">
-        <v>53.72</v>
-      </c>
-      <c r="F14" s="23">
-        <v>350.02</v>
-      </c>
-      <c r="G14" s="23">
-        <v>53.36</v>
-      </c>
-      <c r="H14" s="23">
-        <v>18.36</v>
-      </c>
-      <c r="I14" s="23">
-        <v>42.54</v>
-      </c>
-      <c r="J14" s="23">
-        <v>49.1</v>
-      </c>
-      <c r="K14" s="23">
-        <v>56.15</v>
-      </c>
-      <c r="L14" s="23">
-        <v>82.05</v>
-      </c>
-      <c r="M14" s="23">
-        <v>35.01</v>
-      </c>
-      <c r="N14" s="23">
-        <v>0</v>
-      </c>
-      <c r="O14" s="23">
-        <v>62.13</v>
-      </c>
-      <c r="P14" s="23">
-        <v>342.38</v>
-      </c>
-      <c r="Q14" s="23">
-        <v>49.1</v>
-      </c>
-      <c r="R14" s="23">
-        <v>5.37</v>
-      </c>
-      <c r="S14" s="23">
-        <v>52.47</v>
-      </c>
-      <c r="T14" s="23">
-        <v>53.69</v>
-      </c>
-      <c r="U14" s="23">
-        <v>113.79</v>
-      </c>
-      <c r="V14" s="23">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="29">
-        <v>11</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="23">
-        <v>58.07</v>
-      </c>
-      <c r="E15" s="23">
-        <v>9.02</v>
-      </c>
-      <c r="F15" s="23">
-        <v>394.98</v>
-      </c>
-      <c r="G15" s="23">
-        <v>11.61</v>
-      </c>
-      <c r="H15" s="23">
-        <v>52.02</v>
-      </c>
-      <c r="I15" s="23">
-        <v>66.260000000000005</v>
-      </c>
-      <c r="J15" s="23">
-        <v>72.819999999999993</v>
-      </c>
-      <c r="K15" s="23">
-        <v>79.87</v>
-      </c>
-      <c r="L15" s="23">
-        <v>27.57</v>
-      </c>
-      <c r="M15" s="23">
-        <v>28.24</v>
-      </c>
-      <c r="N15" s="23">
-        <v>63.21</v>
-      </c>
-      <c r="O15" s="23">
-        <v>0</v>
-      </c>
-      <c r="P15" s="23">
-        <v>387.34</v>
-      </c>
-      <c r="Q15" s="23">
-        <v>72.819999999999993</v>
-      </c>
-      <c r="R15" s="23">
-        <v>59.64</v>
-      </c>
-      <c r="S15" s="23">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="T15" s="23">
-        <v>8.6</v>
-      </c>
-      <c r="U15" s="23">
-        <v>163.75</v>
-      </c>
-      <c r="V15" s="23">
-        <v>73.66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="29">
-        <v>12</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="23">
-        <v>337.26</v>
-      </c>
-      <c r="E16" s="23">
-        <v>379.54</v>
-      </c>
-      <c r="F16" s="23">
-        <v>22.6</v>
-      </c>
-      <c r="G16" s="23">
-        <v>375.95</v>
-      </c>
-      <c r="H16" s="23">
-        <v>348.27</v>
-      </c>
-      <c r="I16" s="23">
-        <v>326.01</v>
-      </c>
-      <c r="J16" s="23">
-        <v>319.79000000000002</v>
-      </c>
-      <c r="K16" s="23">
-        <v>312.12</v>
-      </c>
-      <c r="L16" s="23">
-        <v>410.67</v>
-      </c>
-      <c r="M16" s="23">
-        <v>363.63</v>
-      </c>
-      <c r="N16" s="23">
-        <v>342.4</v>
-      </c>
-      <c r="O16" s="23">
-        <v>387.38</v>
-      </c>
-      <c r="P16" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="23">
-        <v>319.79000000000002</v>
-      </c>
-      <c r="R16" s="23">
-        <v>338.83</v>
-      </c>
-      <c r="S16" s="23">
-        <v>378.29</v>
-      </c>
-      <c r="T16" s="23">
-        <v>379.51</v>
-      </c>
-      <c r="U16" s="23">
-        <v>234.98</v>
-      </c>
-      <c r="V16" s="23">
-        <v>311.91000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17" s="29">
-        <v>13</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="23">
-        <v>45.06</v>
-      </c>
-      <c r="E17" s="23">
-        <v>65.77</v>
-      </c>
-      <c r="F17" s="23">
-        <v>327.67</v>
-      </c>
-      <c r="G17" s="23">
-        <v>62.18</v>
-      </c>
-      <c r="H17" s="23">
-        <v>43.65</v>
-      </c>
-      <c r="I17" s="23">
-        <v>7.34</v>
-      </c>
-      <c r="J17" s="23">
-        <v>0</v>
-      </c>
-      <c r="K17" s="23">
-        <v>8.01</v>
-      </c>
-      <c r="L17" s="23">
-        <v>96.9</v>
-      </c>
-      <c r="M17" s="23">
-        <v>49.86</v>
-      </c>
-      <c r="N17" s="23">
-        <v>50.2</v>
-      </c>
-      <c r="O17" s="23">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="P17" s="23">
-        <v>320.02999999999997</v>
-      </c>
-      <c r="Q17" s="23">
-        <v>0</v>
-      </c>
-      <c r="R17" s="23">
-        <v>46.63</v>
-      </c>
-      <c r="S17" s="23">
-        <v>64.510000000000005</v>
-      </c>
-      <c r="T17" s="23">
-        <v>65.73</v>
-      </c>
-      <c r="U17" s="23">
-        <v>101.64</v>
-      </c>
-      <c r="V17" s="23">
-        <v>27.13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
-      <c r="A18" s="29">
-        <v>14</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="23">
-        <v>3.17</v>
-      </c>
-      <c r="E18" s="23">
-        <v>47.52</v>
-      </c>
-      <c r="F18" s="23">
-        <v>346.47</v>
-      </c>
-      <c r="G18" s="23">
-        <v>49.81</v>
-      </c>
-      <c r="H18" s="23">
-        <v>14.79</v>
-      </c>
-      <c r="I18" s="23">
-        <v>38.99</v>
-      </c>
-      <c r="J18" s="23">
-        <v>45.55</v>
-      </c>
-      <c r="K18" s="23">
-        <v>52.6</v>
-      </c>
-      <c r="L18" s="23">
-        <v>76.180000000000007</v>
-      </c>
-      <c r="M18" s="23">
-        <v>31.61</v>
-      </c>
-      <c r="N18" s="23">
-        <v>5.14</v>
-      </c>
-      <c r="O18" s="23">
-        <v>61.24</v>
-      </c>
-      <c r="P18" s="23">
-        <v>338.83</v>
-      </c>
-      <c r="Q18" s="23">
-        <v>45.55</v>
-      </c>
-      <c r="R18" s="23">
-        <v>0</v>
-      </c>
-      <c r="S18" s="23">
-        <v>46.27</v>
-      </c>
-      <c r="T18" s="23">
-        <v>47.49</v>
-      </c>
-      <c r="U18" s="23">
-        <v>110.24</v>
-      </c>
-      <c r="V18" s="23">
-        <v>59.45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="29">
-        <v>15</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="23">
-        <v>44.1</v>
-      </c>
-      <c r="E19" s="23">
-        <v>1.72</v>
-      </c>
-      <c r="F19" s="23">
-        <v>386.88</v>
-      </c>
-      <c r="G19" s="23">
-        <v>11.82</v>
-      </c>
-      <c r="H19" s="23">
-        <v>35.369999999999997</v>
-      </c>
-      <c r="I19" s="23">
-        <v>58.15</v>
-      </c>
-      <c r="J19" s="23">
-        <v>64.709999999999994</v>
-      </c>
-      <c r="K19" s="23">
-        <v>71.760000000000005</v>
-      </c>
-      <c r="L19" s="23">
-        <v>29.13</v>
-      </c>
-      <c r="M19" s="23">
-        <v>17.73</v>
-      </c>
-      <c r="N19" s="23">
-        <v>56.94</v>
-      </c>
-      <c r="O19" s="23">
-        <v>9.58</v>
-      </c>
-      <c r="P19" s="23">
-        <v>379.24</v>
-      </c>
-      <c r="Q19" s="23">
-        <v>64.709999999999994</v>
-      </c>
-      <c r="R19" s="23">
-        <v>46.38</v>
-      </c>
-      <c r="S19" s="23">
-        <v>0</v>
-      </c>
-      <c r="T19" s="23">
-        <v>1.68</v>
-      </c>
-      <c r="U19" s="23">
-        <v>162.63999999999999</v>
-      </c>
-      <c r="V19" s="23">
-        <v>74.48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" s="29">
-        <v>16</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="23">
-        <v>45.51</v>
-      </c>
-      <c r="E20" s="23">
-        <v>0.62</v>
-      </c>
-      <c r="F20" s="23">
-        <v>388.29</v>
-      </c>
-      <c r="G20" s="23">
-        <v>12.28</v>
-      </c>
-      <c r="H20" s="23">
-        <v>36.78</v>
-      </c>
-      <c r="I20" s="23">
-        <v>59.56</v>
-      </c>
-      <c r="J20" s="23">
-        <v>66.12</v>
-      </c>
-      <c r="K20" s="23">
-        <v>73.17</v>
-      </c>
-      <c r="L20" s="23">
-        <v>29.23</v>
-      </c>
-      <c r="M20" s="23">
-        <v>19.14</v>
-      </c>
-      <c r="N20" s="23">
-        <v>57.1</v>
-      </c>
-      <c r="O20" s="23">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="P20" s="23">
-        <v>380.65</v>
-      </c>
-      <c r="Q20" s="23">
-        <v>66.12</v>
-      </c>
-      <c r="R20" s="23">
-        <v>47.79</v>
-      </c>
-      <c r="S20" s="23">
-        <v>1.55</v>
-      </c>
-      <c r="T20" s="23">
-        <v>0</v>
-      </c>
-      <c r="U20" s="23">
-        <v>162.80000000000001</v>
-      </c>
-      <c r="V20" s="23">
-        <v>70.55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
-      <c r="A21" s="29">
-        <v>17</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="23">
-        <v>108.77</v>
-      </c>
-      <c r="E21" s="23">
-        <v>163</v>
-      </c>
-      <c r="F21" s="23">
-        <v>251.96</v>
-      </c>
-      <c r="G21" s="23">
-        <v>153.21</v>
-      </c>
-      <c r="H21" s="23">
-        <v>119.78</v>
-      </c>
-      <c r="I21" s="23">
-        <v>108.25</v>
-      </c>
-      <c r="J21" s="23">
-        <v>102.03</v>
-      </c>
-      <c r="K21" s="23">
-        <v>94.36</v>
-      </c>
-      <c r="L21" s="23">
-        <v>191.33</v>
-      </c>
-      <c r="M21" s="23">
-        <v>136.86000000000001</v>
-      </c>
-      <c r="N21" s="23">
-        <v>113.91</v>
-      </c>
-      <c r="O21" s="23">
-        <v>164.64</v>
-      </c>
-      <c r="P21" s="23">
-        <v>235.16</v>
-      </c>
-      <c r="Q21" s="23">
-        <v>102.03</v>
-      </c>
-      <c r="R21" s="23">
-        <v>110.34</v>
-      </c>
-      <c r="S21" s="23">
-        <v>161.75</v>
-      </c>
-      <c r="T21" s="23">
-        <v>162.97</v>
-      </c>
-      <c r="U21" s="23">
-        <v>0</v>
-      </c>
-      <c r="V21" s="23">
-        <v>120.34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="A22" s="29">
-        <v>18</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="23">
+      <c r="D22" s="45">
         <v>57.59</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="45">
         <v>72.989999999999995</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="45">
         <v>320.5</v>
       </c>
-      <c r="G22" s="23">
+      <c r="G22" s="45">
         <v>63.03</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="45">
         <v>56.18</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="45">
         <v>34.83</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="45">
         <v>24.37</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="45">
         <v>25.11</v>
       </c>
-      <c r="L22" s="23">
+      <c r="L22" s="45">
         <v>101.62</v>
       </c>
-      <c r="M22" s="23">
+      <c r="M22" s="45">
         <v>62.39</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="45">
         <v>62.73</v>
       </c>
-      <c r="O22" s="23">
+      <c r="O22" s="45">
         <v>75.010000000000005</v>
       </c>
-      <c r="P22" s="23">
+      <c r="P22" s="45">
         <v>312.86</v>
       </c>
-      <c r="Q22" s="23">
+      <c r="Q22" s="45">
         <v>24.37</v>
       </c>
-      <c r="R22" s="23">
+      <c r="R22" s="45">
         <v>59.16</v>
       </c>
-      <c r="S22" s="23">
+      <c r="S22" s="45">
         <v>71.739999999999995</v>
       </c>
-      <c r="T22" s="23">
+      <c r="T22" s="45">
         <v>72.959999999999994</v>
       </c>
-      <c r="U22" s="23">
+      <c r="U22" s="45">
         <v>120.47</v>
       </c>
-      <c r="V22" s="23">
+      <c r="V22" s="45">
         <v>0</v>
       </c>
     </row>
@@ -3390,20 +3384,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" style="23" customWidth="1"/>
-    <col min="2" max="6" width="8.86328125" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="8.86328125" style="23"/>
+    <col min="1" max="1" width="26.453125" style="23" customWidth="1"/>
+    <col min="2" max="6" width="8.81640625" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.95" customHeight="1">
+    <row r="1" spans="1:5" ht="16" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3416,11 +3410,11 @@
       <c r="D1" s="3"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1">
+    <row r="2" spans="1:5" ht="16" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="36">
+        <v>71</v>
+      </c>
+      <c r="B2" s="32">
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -3429,9 +3423,9 @@
       <c r="D2" s="5"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+    <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B3" s="6">
         <v>80</v>
@@ -3442,11 +3436,11 @@
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" ht="15.95" customHeight="1">
+    <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="40">
+        <v>73</v>
+      </c>
+      <c r="B4" s="35">
         <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -3455,12 +3449,12 @@
       <c r="D4" s="5"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="15.95" customHeight="1">
+    <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="40">
-        <v>15</v>
+      <c r="B5" s="35">
+        <v>30</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>6</v>
@@ -3468,11 +3462,11 @@
       <c r="D5" s="5"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="15.95" customHeight="1">
+    <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="36">
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -3484,50 +3478,30 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A7" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="42">
+      <c r="A7" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="37">
         <v>30</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="34" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A8" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="38">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>73</v>
+      <c r="A8" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="37">
+        <v>0</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>6</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A9" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="38">
-        <v>0.625</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A10" s="43"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3542,30 +3516,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C15"/>
+    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" customWidth="1"/>
-    <col min="2" max="2" width="20.3984375" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" customWidth="1"/>
-    <col min="4" max="6" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1">
+    <row r="2" spans="1:3" ht="16" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -3576,7 +3550,7 @@
         <v>6561</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1">
+    <row r="3" spans="1:3" ht="16" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -3587,7 +3561,7 @@
         <v>6561</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1">
+    <row r="4" spans="1:3" ht="16" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -3598,7 +3572,7 @@
         <v>6561</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1">
+    <row r="5" spans="1:3" ht="16" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -3609,7 +3583,7 @@
         <v>8366</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.95" customHeight="1">
+    <row r="6" spans="1:3" ht="16" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -3620,7 +3594,7 @@
         <v>8366</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.95" customHeight="1">
+    <row r="7" spans="1:3" ht="16" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -3631,7 +3605,7 @@
         <v>8366</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.95" customHeight="1">
+    <row r="8" spans="1:3" ht="16" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
@@ -3642,7 +3616,7 @@
         <v>10344</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.95" customHeight="1">
+    <row r="9" spans="1:3" ht="16" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>19</v>
       </c>
@@ -3653,7 +3627,7 @@
         <v>10344</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.95" customHeight="1">
+    <row r="10" spans="1:3" ht="16" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -3664,7 +3638,7 @@
         <v>12278</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.95" customHeight="1">
+    <row r="11" spans="1:3" ht="16" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
@@ -3675,7 +3649,7 @@
         <v>12278</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.95" customHeight="1">
+    <row r="12" spans="1:3" ht="16" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
@@ -3686,7 +3660,7 @@
         <v>17129</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.95" customHeight="1">
+    <row r="13" spans="1:3" ht="16" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
@@ -3722,19 +3696,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.265625" customWidth="1"/>
-    <col min="2" max="2" width="36.265625" customWidth="1"/>
-    <col min="3" max="3" width="13.1328125" customWidth="1"/>
-    <col min="4" max="6" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" customHeight="1">
+    <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
@@ -3745,7 +3719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1">
+    <row r="2" spans="1:3" ht="16" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
@@ -3756,199 +3730,199 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1">
+    <row r="3" spans="1:3" ht="16" customHeight="1">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="13">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1">
+    <row r="4" spans="1:3" ht="16" customHeight="1">
       <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="13">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1">
+    <row r="5" spans="1:3" ht="16" customHeight="1">
       <c r="A5" s="14">
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="13">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.95" customHeight="1">
+    <row r="6" spans="1:3" ht="16" customHeight="1">
       <c r="A6" s="14">
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="13">
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.95" customHeight="1">
+    <row r="7" spans="1:3" ht="16" customHeight="1">
       <c r="A7" s="14">
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="13">
         <v>1250</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.95" customHeight="1">
+    <row r="8" spans="1:3" ht="16" customHeight="1">
       <c r="A8" s="14">
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="13">
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.95" customHeight="1">
+    <row r="9" spans="1:3" ht="16" customHeight="1">
       <c r="A9" s="14">
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="13">
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.95" customHeight="1">
+    <row r="10" spans="1:3" ht="16" customHeight="1">
       <c r="A10" s="14">
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="13">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.95" customHeight="1">
+    <row r="11" spans="1:3" ht="16" customHeight="1">
       <c r="A11" s="14">
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="13">
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.95" customHeight="1">
+    <row r="12" spans="1:3" ht="16" customHeight="1">
       <c r="A12" s="14">
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="13">
         <v>1500</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.95" customHeight="1">
+    <row r="13" spans="1:3" ht="16" customHeight="1">
       <c r="A13" s="14">
         <v>11</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="13">
         <v>3500</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.95" customHeight="1">
+    <row r="14" spans="1:3" ht="16" customHeight="1">
       <c r="A14" s="14">
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="13">
         <v>2500</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.95" customHeight="1">
+    <row r="15" spans="1:3" ht="16" customHeight="1">
       <c r="A15" s="14">
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="13">
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.95" customHeight="1">
+    <row r="16" spans="1:3" ht="16" customHeight="1">
       <c r="A16" s="14">
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="13">
         <v>3000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.95" customHeight="1">
+    <row r="17" spans="1:3" ht="16" customHeight="1">
       <c r="A17" s="14">
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="13">
         <v>3000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.95" customHeight="1">
+    <row r="18" spans="1:3" ht="16" customHeight="1">
       <c r="A18" s="14">
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="13">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.95" customHeight="1">
+    <row r="19" spans="1:3" ht="16" customHeight="1">
       <c r="A19" s="14">
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="13">
         <v>4000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.95" customHeight="1">
+    <row r="20" spans="1:3" ht="16" customHeight="1">
       <c r="A20" s="14">
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="13">
         <v>8000</v>
@@ -3967,340 +3941,340 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.265625" customWidth="1"/>
-    <col min="2" max="2" width="36.265625" customWidth="1"/>
-    <col min="3" max="3" width="26.86328125" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.86328125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.95" customHeight="1">
+    <row r="1" spans="1:5" ht="16" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E1" s="40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1">
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="45">
+      <c r="B2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="39">
         <v>2.375</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="42">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="41">
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.95" customHeight="1">
+    <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="45">
+        <v>34</v>
+      </c>
+      <c r="C3" s="39">
         <v>2.375</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="42">
         <v>0.75</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="41">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.95" customHeight="1">
+    <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="45">
+        <v>35</v>
+      </c>
+      <c r="C4" s="39">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.95" customHeight="1">
+    <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="45">
+        <v>36</v>
+      </c>
+      <c r="C5" s="39">
         <v>2.375</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="42">
         <v>0.75</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="41">
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.95" customHeight="1">
+    <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="45">
+        <v>37</v>
+      </c>
+      <c r="C6" s="39">
         <v>2.375</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="42">
         <v>0.75</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.95" customHeight="1">
+    <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="45">
+        <v>38</v>
+      </c>
+      <c r="C7" s="39">
         <v>2.375</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="42">
         <v>0.75</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.95" customHeight="1">
+    <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="45">
+        <v>39</v>
+      </c>
+      <c r="C8" s="39">
         <v>2.375</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="42">
         <v>0.75</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.95" customHeight="1">
+    <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="45">
+        <v>40</v>
+      </c>
+      <c r="C9" s="39">
         <v>2.375</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="42">
         <v>0.75</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.95" customHeight="1">
+    <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="45">
+        <v>41</v>
+      </c>
+      <c r="C10" s="39">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="42">
         <v>0.75</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.95" customHeight="1">
+    <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" s="14">
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="45">
+        <v>42</v>
+      </c>
+      <c r="C11" s="39">
         <v>2.375</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="42">
         <v>0.75</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.95" customHeight="1">
+    <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" s="14">
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="45">
+        <v>43</v>
+      </c>
+      <c r="C12" s="39">
         <v>2.375</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="42">
         <v>0.75</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="41">
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.95" customHeight="1">
+    <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" s="14">
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="45">
+        <v>44</v>
+      </c>
+      <c r="C13" s="39">
         <v>2.375</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="42">
         <v>0.75</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.95" customHeight="1">
+    <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" s="14">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="45">
+        <v>45</v>
+      </c>
+      <c r="C14" s="39">
         <v>2.375</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="42">
         <v>0.75</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1">
+    <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" s="14">
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="45">
+        <v>46</v>
+      </c>
+      <c r="C15" s="39">
         <v>2.375</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="42">
         <v>0.75</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.95" customHeight="1">
+    <row r="16" spans="1:5" ht="16" customHeight="1">
       <c r="A16" s="14">
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="45">
+        <v>47</v>
+      </c>
+      <c r="C16" s="39">
         <v>2.375</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="42">
         <v>0.75</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="41">
         <v>3500</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.95" customHeight="1">
+    <row r="17" spans="1:5" ht="16" customHeight="1">
       <c r="A17" s="14">
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="45">
+        <v>48</v>
+      </c>
+      <c r="C17" s="39">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="42">
         <v>0.75</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.95" customHeight="1">
+    <row r="18" spans="1:5" ht="16" customHeight="1">
       <c r="A18" s="14">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="45">
+        <v>49</v>
+      </c>
+      <c r="C18" s="39">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="42">
         <v>0.75</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="41">
         <v>11000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.95" customHeight="1">
+    <row r="19" spans="1:5" ht="16" customHeight="1">
       <c r="A19" s="14">
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="45">
+        <v>50</v>
+      </c>
+      <c r="C19" s="39">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="42">
         <v>0.6875</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="41">
         <v>11000</v>
       </c>
     </row>
@@ -4320,22 +4294,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.3984375" defaultRowHeight="14.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="23.453125" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.1328125" customWidth="1"/>
-    <col min="2" max="2" width="27.73046875" customWidth="1"/>
-    <col min="3" max="20" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.3984375" customWidth="1"/>
-    <col min="22" max="22" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" customWidth="1"/>
+    <col min="3" max="20" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.95" customHeight="1">
+    <row r="1" spans="1:21" ht="16" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
@@ -4345,7 +4318,7 @@
       <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="27">
+      <c r="D1" s="26">
         <v>1</v>
       </c>
       <c r="E1" s="16">
@@ -4400,77 +4373,97 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.95" customHeight="1">
+    <row r="2" spans="1:21" ht="16" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.95" customHeight="1">
+      <c r="C2" s="43" t="str" cm="1">
+        <f t="array" ref="C2">IF(ISBLANK(C$1),"",_xlfn.XLOOKUP(C$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>Osan DC</v>
+      </c>
+      <c r="D2" s="43" t="str" cm="1">
+        <f t="array" ref="D2">IF(ISBLANK(D$1),"",_xlfn.XLOOKUP(D$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>이솝(금천가산)</v>
+      </c>
+      <c r="E2" s="43" t="str" cm="1">
+        <f t="array" ref="E2">IF(ISBLANK(E$1),"",_xlfn.XLOOKUP(E$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>보조기전(부산사상괘법)</v>
+      </c>
+      <c r="F2" s="43" t="str" cm="1">
+        <f t="array" ref="F2">IF(ISBLANK(F$1),"",_xlfn.XLOOKUP(F$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>대현시그마(서초방배)</v>
+      </c>
+      <c r="G2" s="43" t="str" cm="1">
+        <f t="array" ref="G2">IF(ISBLANK(G$1),"",_xlfn.XLOOKUP(G$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>다스코리아(화성기산)</v>
+      </c>
+      <c r="H2" s="43" t="str" cm="1">
+        <f t="array" ref="H2">IF(ISBLANK(H$1),"",_xlfn.XLOOKUP(H$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>에티버스(용인처인)</v>
+      </c>
+      <c r="I2" s="43" t="str" cm="1">
+        <f t="array" ref="I2">IF(ISBLANK(I$1),"",_xlfn.XLOOKUP(I$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>에티버스이앤엘(용인백봉)</v>
+      </c>
+      <c r="J2" s="43" t="str" cm="1">
+        <f t="array" ref="J2">IF(ISBLANK(J$1),"",_xlfn.XLOOKUP(J$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>근우(안성죽산)</v>
+      </c>
+      <c r="K2" s="43" t="str" cm="1">
+        <f t="array" ref="K2">IF(ISBLANK(K$1),"",_xlfn.XLOOKUP(K$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>인택(인천서구)</v>
+      </c>
+      <c r="L2" s="43" t="str" cm="1">
+        <f t="array" ref="L2">IF(ISBLANK(L$1),"",_xlfn.XLOOKUP(L$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>진주일렉콤(군포당정)</v>
+      </c>
+      <c r="M2" s="43" t="str" cm="1">
+        <f t="array" ref="M2">IF(ISBLANK(M$1),"",_xlfn.XLOOKUP(M$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>조일물류(평택서탄)</v>
+      </c>
+      <c r="N2" s="43" t="str" cm="1">
+        <f t="array" ref="N2">IF(ISBLANK(N$1),"",_xlfn.XLOOKUP(N$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>제이에스시스템(안성공도용두)</v>
+      </c>
+      <c r="O2" s="43" t="str" cm="1">
+        <f t="array" ref="O2">IF(ISBLANK(O$1),"",_xlfn.XLOOKUP(O$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>KTE(부산강서)</v>
+      </c>
+      <c r="P2" s="43" t="str" cm="1">
+        <f t="array" ref="P2">IF(ISBLANK(P$1),"",_xlfn.XLOOKUP(P$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>로지비스(용인백봉)</v>
+      </c>
+      <c r="Q2" s="43" t="str" cm="1">
+        <f t="array" ref="Q2">IF(ISBLANK(Q$1),"",_xlfn.XLOOKUP(Q$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>알에스오토메이션(평택진위)</v>
+      </c>
+      <c r="R2" s="43" t="str" cm="1">
+        <f t="array" ref="R2">IF(ISBLANK(R$1),"",_xlfn.XLOOKUP(R$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>서광엔비에이(금천가산)</v>
+      </c>
+      <c r="S2" s="43" t="str" cm="1">
+        <f t="array" ref="S2">IF(ISBLANK(S$1),"",_xlfn.XLOOKUP(S$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>세림디티에스(금천가산)</v>
+      </c>
+      <c r="T2" s="43" t="str" cm="1">
+        <f t="array" ref="T2">IF(ISBLANK(T$1),"",_xlfn.XLOOKUP(T$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>유니템(화성영천)</v>
+      </c>
+      <c r="U2" s="43" t="str" cm="1">
+        <f t="array" ref="U2">IF(ISBLANK(U$1),"",_xlfn.XLOOKUP(U$1,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>발렉스코리아(이천부발)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="16" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>31</v>
+      <c r="B3" s="43" t="str" cm="1">
+        <f t="array" ref="B3">IF(ISBLANK($A3),"",_xlfn.XLOOKUP($A3,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>Osan DC</v>
       </c>
       <c r="C3" s="18" cm="1">
         <f t="array" ref="C3">_xlfn.XLOOKUP($A3,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -4549,12 +4542,13 @@
         <v>57.92</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.95" customHeight="1">
-      <c r="A4" s="27">
+    <row r="4" spans="1:21" ht="16" customHeight="1">
+      <c r="A4" s="26">
         <v>1</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>35</v>
+      <c r="B4" s="43" t="str" cm="1">
+        <f t="array" ref="B4">IF(ISBLANK($A4),"",_xlfn.XLOOKUP($A4,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>이솝(금천가산)</v>
       </c>
       <c r="C4" s="18" cm="1">
         <f t="array" ref="C4">_xlfn.XLOOKUP($A4,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -4633,12 +4627,13 @@
         <v>70.55</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.95" customHeight="1">
+    <row r="5" spans="1:21" ht="16" customHeight="1">
       <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>36</v>
+      <c r="B5" s="43" t="str" cm="1">
+        <f t="array" ref="B5">IF(ISBLANK($A5),"",_xlfn.XLOOKUP($A5,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>보조기전(부산사상괘법)</v>
       </c>
       <c r="C5" s="18" cm="1">
         <f t="array" ref="C5">_xlfn.XLOOKUP($A5,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -4717,12 +4712,13 @@
         <v>320.35000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.95" customHeight="1">
+    <row r="6" spans="1:21" ht="16" customHeight="1">
       <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
+      <c r="B6" s="43" t="str" cm="1">
+        <f t="array" ref="B6">IF(ISBLANK($A6),"",_xlfn.XLOOKUP($A6,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>대현시그마(서초방배)</v>
       </c>
       <c r="C6" s="18" cm="1">
         <f t="array" ref="C6">_xlfn.XLOOKUP($A6,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -4801,12 +4797,13 @@
         <v>62.91</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.95" customHeight="1">
+    <row r="7" spans="1:21" ht="16" customHeight="1">
       <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>38</v>
+      <c r="B7" s="43" t="str" cm="1">
+        <f t="array" ref="B7">IF(ISBLANK($A7),"",_xlfn.XLOOKUP($A7,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>다스코리아(화성기산)</v>
       </c>
       <c r="C7" s="18" cm="1">
         <f t="array" ref="C7">_xlfn.XLOOKUP($A7,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -4885,12 +4882,13 @@
         <v>56.61</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.95" customHeight="1">
+    <row r="8" spans="1:21" ht="16" customHeight="1">
       <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>39</v>
+      <c r="B8" s="43" t="str" cm="1">
+        <f t="array" ref="B8">IF(ISBLANK($A8),"",_xlfn.XLOOKUP($A8,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>에티버스(용인처인)</v>
       </c>
       <c r="C8" s="18" cm="1">
         <f t="array" ref="C8">_xlfn.XLOOKUP($A8,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -4969,12 +4967,13 @@
         <v>35.29</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.95" customHeight="1">
+    <row r="9" spans="1:21" ht="16" customHeight="1">
       <c r="A9" s="16">
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>40</v>
+      <c r="B9" s="43" t="str" cm="1">
+        <f t="array" ref="B9">IF(ISBLANK($A9),"",_xlfn.XLOOKUP($A9,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>에티버스이앤엘(용인백봉)</v>
       </c>
       <c r="C9" s="18" cm="1">
         <f t="array" ref="C9">_xlfn.XLOOKUP($A9,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5053,12 +5052,13 @@
         <v>27.13</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.95" customHeight="1">
+    <row r="10" spans="1:21" ht="16" customHeight="1">
       <c r="A10" s="16">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>41</v>
+      <c r="B10" s="43" t="str" cm="1">
+        <f t="array" ref="B10">IF(ISBLANK($A10),"",_xlfn.XLOOKUP($A10,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>근우(안성죽산)</v>
       </c>
       <c r="C10" s="18" cm="1">
         <f t="array" ref="C10">_xlfn.XLOOKUP($A10,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5137,12 +5137,13 @@
         <v>24.97</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.95" customHeight="1">
+    <row r="11" spans="1:21" ht="16" customHeight="1">
       <c r="A11" s="16">
         <v>8</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>42</v>
+      <c r="B11" s="43" t="str" cm="1">
+        <f t="array" ref="B11">IF(ISBLANK($A11),"",_xlfn.XLOOKUP($A11,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>인택(인천서구)</v>
       </c>
       <c r="C11" s="18" cm="1">
         <f t="array" ref="C11">_xlfn.XLOOKUP($A11,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5221,12 +5222,13 @@
         <v>98.16</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.95" customHeight="1">
+    <row r="12" spans="1:21" ht="16" customHeight="1">
       <c r="A12" s="16">
         <v>9</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>43</v>
+      <c r="B12" s="43" t="str" cm="1">
+        <f t="array" ref="B12">IF(ISBLANK($A12),"",_xlfn.XLOOKUP($A12,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>진주일렉콤(군포당정)</v>
       </c>
       <c r="C12" s="18" cm="1">
         <f t="array" ref="C12">_xlfn.XLOOKUP($A12,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5305,12 +5307,13 @@
         <v>63.85</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.95" customHeight="1">
+    <row r="13" spans="1:21" ht="16" customHeight="1">
       <c r="A13" s="16">
         <v>10</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>44</v>
+      <c r="B13" s="43" t="str" cm="1">
+        <f t="array" ref="B13">IF(ISBLANK($A13),"",_xlfn.XLOOKUP($A13,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>조일물류(평택서탄)</v>
       </c>
       <c r="C13" s="18" cm="1">
         <f t="array" ref="C13">_xlfn.XLOOKUP($A13,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5389,12 +5392,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.95" customHeight="1">
+    <row r="14" spans="1:21" ht="16" customHeight="1">
       <c r="A14" s="16">
         <v>11</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>45</v>
+      <c r="B14" s="43" t="str" cm="1">
+        <f t="array" ref="B14">IF(ISBLANK($A14),"",_xlfn.XLOOKUP($A14,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>제이에스시스템(안성공도용두)</v>
       </c>
       <c r="C14" s="18" cm="1">
         <f t="array" ref="C14">_xlfn.XLOOKUP($A14,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5473,12 +5477,13 @@
         <v>73.66</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.95" customHeight="1">
+    <row r="15" spans="1:21" ht="16" customHeight="1">
       <c r="A15" s="16">
         <v>12</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>46</v>
+      <c r="B15" s="43" t="str" cm="1">
+        <f t="array" ref="B15">IF(ISBLANK($A15),"",_xlfn.XLOOKUP($A15,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>KTE(부산강서)</v>
       </c>
       <c r="C15" s="18" cm="1">
         <f t="array" ref="C15">_xlfn.XLOOKUP($A15,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5557,12 +5562,13 @@
         <v>311.91000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.95" customHeight="1">
+    <row r="16" spans="1:21" ht="16" customHeight="1">
       <c r="A16" s="16">
         <v>13</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>47</v>
+      <c r="B16" s="43" t="str" cm="1">
+        <f t="array" ref="B16">IF(ISBLANK($A16),"",_xlfn.XLOOKUP($A16,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>로지비스(용인백봉)</v>
       </c>
       <c r="C16" s="18" cm="1">
         <f t="array" ref="C16">_xlfn.XLOOKUP($A16,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5641,12 +5647,13 @@
         <v>27.13</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.95" customHeight="1">
+    <row r="17" spans="1:21" ht="16" customHeight="1">
       <c r="A17" s="16">
         <v>14</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>48</v>
+      <c r="B17" s="43" t="str" cm="1">
+        <f t="array" ref="B17">IF(ISBLANK($A17),"",_xlfn.XLOOKUP($A17,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>알에스오토메이션(평택진위)</v>
       </c>
       <c r="C17" s="18" cm="1">
         <f t="array" ref="C17">_xlfn.XLOOKUP($A17,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5725,12 +5732,13 @@
         <v>59.45</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.95" customHeight="1">
+    <row r="18" spans="1:21" ht="16" customHeight="1">
       <c r="A18" s="16">
         <v>15</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>49</v>
+      <c r="B18" s="43" t="str" cm="1">
+        <f t="array" ref="B18">IF(ISBLANK($A18),"",_xlfn.XLOOKUP($A18,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>서광엔비에이(금천가산)</v>
       </c>
       <c r="C18" s="18" cm="1">
         <f t="array" ref="C18">_xlfn.XLOOKUP($A18,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5809,12 +5817,13 @@
         <v>74.48</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.95" customHeight="1">
+    <row r="19" spans="1:21" ht="16" customHeight="1">
       <c r="A19" s="16">
         <v>16</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>50</v>
+      <c r="B19" s="43" t="str" cm="1">
+        <f t="array" ref="B19">IF(ISBLANK($A19),"",_xlfn.XLOOKUP($A19,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>세림디티에스(금천가산)</v>
       </c>
       <c r="C19" s="18" cm="1">
         <f t="array" ref="C19">_xlfn.XLOOKUP($A19,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5893,12 +5902,13 @@
         <v>70.55</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.95" customHeight="1">
+    <row r="20" spans="1:21" ht="16" customHeight="1">
       <c r="A20" s="16">
         <v>17</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>51</v>
+      <c r="B20" s="43" t="str" cm="1">
+        <f t="array" ref="B20">IF(ISBLANK($A20),"",_xlfn.XLOOKUP($A20,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>유니템(화성영천)</v>
       </c>
       <c r="C20" s="18" cm="1">
         <f t="array" ref="C20">_xlfn.XLOOKUP($A20,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -5977,12 +5987,13 @@
         <v>120.34</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.95" customHeight="1">
+    <row r="21" spans="1:21" ht="16" customHeight="1">
       <c r="A21" s="16">
         <v>18</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>52</v>
+      <c r="B21" s="43" t="str" cm="1">
+        <f t="array" ref="B21">IF(ISBLANK($A21),"",_xlfn.XLOOKUP($A21,_xlfn._TRO_ALL('Distance Database'!$A:$A),_xlfn._TRO_ALL('Distance Database'!$B:$B),"Not Found",0))</f>
+        <v>발렉스코리아(이천부발)</v>
       </c>
       <c r="C21" s="18" cm="1">
         <f t="array" ref="C21">_xlfn.XLOOKUP($A21,'Distance Database'!$A:$A,_xlfn.XLOOKUP(C$1,'Distance Database'!$1:$1,'Distance Database'!$1:$1048576))</f>
@@ -6061,42 +6072,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="14.25" customHeight="1">
-      <c r="G24" s="35"/>
+    <row r="23" spans="1:21" ht="14.25" customHeight="1">
+      <c r="G23" s="31"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>A$1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD2">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>A$2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$B1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:U1">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:U2">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6109,6 +6120,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="49d2c78d-72af-4bb0-ba0a-682023aa8426" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="78e9dec5-09ed-416b-9c6b-b596d250c427">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010017AB72F0B315504B9A79DD25F871610D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="081d5fb8dfe787f6799543198c60e602">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78e9dec5-09ed-416b-9c6b-b596d250c427" xmlns:ns3="49d2c78d-72af-4bb0-ba0a-682023aa8426" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd7832f611d3e6cdc1a1982cdfae96f7" ns2:_="" ns3:_="">
     <xsd:import namespace="78e9dec5-09ed-416b-9c6b-b596d250c427"/>
@@ -6303,27 +6334,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD6A542E-BBA0-4448-85A0-F092D8CEC56E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="49d2c78d-72af-4bb0-ba0a-682023aa8426" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="78e9dec5-09ed-416b-9c6b-b596d250c427">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43EEAA4C-1740-45E4-AB56-30BCC6AC325E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="49d2c78d-72af-4bb0-ba0a-682023aa8426"/>
+    <ds:schemaRef ds:uri="78e9dec5-09ed-416b-9c6b-b596d250c427"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AED4EF5-9CE8-4B6B-8BE0-93EA92108D9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6340,23 +6370,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD6A542E-BBA0-4448-85A0-F092D8CEC56E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43EEAA4C-1740-45E4-AB56-30BCC6AC325E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49d2c78d-72af-4bb0-ba0a-682023aa8426"/>
-    <ds:schemaRef ds:uri="78e9dec5-09ed-416b-9c6b-b596d250c427"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>